<commit_message>
Add curve analysis design doc
</commit_message>
<xml_diff>
--- a/design/cards.xlsx
+++ b/design/cards.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zoey\git\open-card-game\card-design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zoey\git\hexal-ccg\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48877847-76C6-44F6-AAA1-ADCC66CCB1AD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9254A2-CA88-4745-AD8A-FA4CB51CA3C7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="6216" windowWidth="27312" windowHeight="18684" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="384" yWindow="6324" windowWidth="27312" windowHeight="18684" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cards" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="418">
   <si>
     <t>ID</t>
   </si>
@@ -658,9 +658,6 @@
     <t>Resistance</t>
   </si>
   <si>
-    <t>Enchant a friendly creature. It gains +0 / +1. When the creature is destroyed, return this to your hand.</t>
-  </si>
-  <si>
     <t>Mage Armour</t>
   </si>
   <si>
@@ -1289,6 +1286,9 @@
   </si>
   <si>
     <t>Equip to a friendly creature. After combat with an enemy creature, destroy this and the enemy creature.</t>
+  </si>
+  <si>
+    <t>Enchant a friendly creature. It gains +0 / +1. When the creature is destroyed, you may pay [Any] to return this to your hand.</t>
   </si>
 </sst>
 </file>
@@ -1822,11 +1822,6 @@
   <dxfs count="3">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1861,6 +1856,11 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1879,15 +1879,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>4870940</xdr:colOff>
-      <xdr:row>101</xdr:row>
-      <xdr:rowOff>28718</xdr:rowOff>
+      <xdr:colOff>4859217</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>46302</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>6699740</xdr:colOff>
-      <xdr:row>110</xdr:row>
-      <xdr:rowOff>76201</xdr:rowOff>
+      <xdr:colOff>6688017</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>93785</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
@@ -1923,7 +1923,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="10808678" y="2390918"/>
+              <a:off x="10796955" y="2953625"/>
               <a:ext cx="1828800" cy="1682852"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1957,15 +1957,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>5115364</xdr:colOff>
-      <xdr:row>89</xdr:row>
-      <xdr:rowOff>32822</xdr:rowOff>
+      <xdr:colOff>4869179</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>3514</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>109610</xdr:colOff>
-      <xdr:row>96</xdr:row>
-      <xdr:rowOff>175845</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>6697979</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>146538</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
@@ -2001,7 +2001,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="11053102" y="214530"/>
+              <a:off x="10806917" y="1457176"/>
               <a:ext cx="1828800" cy="1414977"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2067,16 +2067,16 @@
   <autoFilter ref="A1:I192" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="2">
       <filters>
-        <filter val="Water"/>
+        <filter val="Fire"/>
       </filters>
     </filterColumn>
   </autoFilter>
   <sortState ref="A2:I192">
     <sortCondition ref="C2:C192" customList="Earth,Fire,Water,Air,Spirit"/>
     <sortCondition ref="D2:D192" customList="Hero,Creature,Spell,Item"/>
-    <sortCondition sortBy="fontColor" ref="F2:F192" dxfId="2"/>
+    <sortCondition sortBy="fontColor" ref="F2:F192" dxfId="1"/>
     <sortCondition ref="F2:F192"/>
-    <sortCondition sortBy="fontColor" ref="E2:E192" dxfId="1"/>
+    <sortCondition sortBy="fontColor" ref="E2:E192" dxfId="0"/>
     <sortCondition ref="E2:E192" customList="Reaction,Enchantment,Equipment,Permanent,Field"/>
     <sortCondition ref="B2:B192"/>
   </sortState>
@@ -2395,7 +2395,7 @@
   <dimension ref="A1:I192"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2485,7 +2485,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
@@ -2500,7 +2500,7 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -2629,7 +2629,7 @@
         <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -2655,7 +2655,7 @@
         <v>11</v>
       </c>
       <c r="F11" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G11">
         <v>2</v>
@@ -2678,7 +2678,7 @@
         <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -2704,7 +2704,7 @@
         <v>11</v>
       </c>
       <c r="F13" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -2747,7 +2747,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C15" t="s">
         <v>10</v>
@@ -2756,7 +2756,7 @@
         <v>11</v>
       </c>
       <c r="F15" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G15">
         <v>3</v>
@@ -2765,7 +2765,7 @@
         <v>4</v>
       </c>
       <c r="I15" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -2773,7 +2773,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C16" t="s">
         <v>10</v>
@@ -2791,7 +2791,7 @@
         <v>2</v>
       </c>
       <c r="I16" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -2799,7 +2799,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C17" t="s">
         <v>10</v>
@@ -2808,7 +2808,7 @@
         <v>11</v>
       </c>
       <c r="F17" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G17">
         <v>2</v>
@@ -2834,7 +2834,7 @@
         <v>11</v>
       </c>
       <c r="F18" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G18">
         <v>3</v>
@@ -2857,7 +2857,7 @@
         <v>11</v>
       </c>
       <c r="F19" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G19">
         <v>2</v>
@@ -2909,7 +2909,7 @@
         <v>11</v>
       </c>
       <c r="F21" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G21">
         <v>3</v>
@@ -2932,7 +2932,7 @@
         <v>11</v>
       </c>
       <c r="F22" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="G22">
         <v>4</v>
@@ -2958,7 +2958,7 @@
         <v>11</v>
       </c>
       <c r="F23" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G23">
         <v>4</v>
@@ -3044,7 +3044,7 @@
         <v>20</v>
       </c>
       <c r="I27" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -3104,7 +3104,7 @@
         <v>17</v>
       </c>
       <c r="I30" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -3127,7 +3127,7 @@
         <v>17</v>
       </c>
       <c r="I31" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -3135,7 +3135,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C32" t="s">
         <v>10</v>
@@ -3155,7 +3155,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C33" t="s">
         <v>10</v>
@@ -3164,10 +3164,10 @@
         <v>15</v>
       </c>
       <c r="F33" t="s">
+        <v>372</v>
+      </c>
+      <c r="I33" t="s">
         <v>373</v>
-      </c>
-      <c r="I33" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -3175,7 +3175,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C34" t="s">
         <v>10</v>
@@ -3184,10 +3184,10 @@
         <v>15</v>
       </c>
       <c r="F34" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I34" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -3250,7 +3250,7 @@
         <v>20</v>
       </c>
       <c r="F37" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="I37" t="s">
         <v>58</v>
@@ -3313,7 +3313,7 @@
         <v>41</v>
       </c>
       <c r="I40" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -3376,10 +3376,10 @@
         <v>17</v>
       </c>
       <c r="I43" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42</v>
       </c>
@@ -3399,7 +3399,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>43</v>
       </c>
@@ -3419,7 +3419,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>44</v>
       </c>
@@ -3442,7 +3442,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>45</v>
       </c>
@@ -3462,7 +3462,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>46</v>
       </c>
@@ -3485,7 +3485,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>47</v>
       </c>
@@ -3505,10 +3505,10 @@
         <v>1</v>
       </c>
       <c r="I49" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>48</v>
       </c>
@@ -3522,7 +3522,7 @@
         <v>11</v>
       </c>
       <c r="F50" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G50">
         <v>1</v>
@@ -3534,7 +3534,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>49</v>
       </c>
@@ -3557,10 +3557,10 @@
         <v>1</v>
       </c>
       <c r="I51" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>50</v>
       </c>
@@ -3583,12 +3583,12 @@
         <v>200</v>
       </c>
     </row>
-    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C53" t="s">
         <v>68</v>
@@ -3606,10 +3606,10 @@
         <v>3</v>
       </c>
       <c r="I53" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>52</v>
       </c>
@@ -3623,7 +3623,7 @@
         <v>11</v>
       </c>
       <c r="F54" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G54">
         <v>2</v>
@@ -3632,7 +3632,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>53</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>11</v>
       </c>
       <c r="F55" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G55">
         <v>4</v>
@@ -3655,7 +3655,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>54</v>
       </c>
@@ -3669,7 +3669,7 @@
         <v>11</v>
       </c>
       <c r="F56" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G56">
         <v>3</v>
@@ -3681,7 +3681,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>55</v>
       </c>
@@ -3707,7 +3707,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>56</v>
       </c>
@@ -3733,7 +3733,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>57</v>
       </c>
@@ -3747,7 +3747,7 @@
         <v>11</v>
       </c>
       <c r="F59" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G59">
         <v>3</v>
@@ -3759,7 +3759,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>58</v>
       </c>
@@ -3785,7 +3785,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>59</v>
       </c>
@@ -3802,7 +3802,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>60</v>
       </c>
@@ -3819,7 +3819,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>61</v>
       </c>
@@ -3839,7 +3839,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>62</v>
       </c>
@@ -3859,7 +3859,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="65" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>63</v>
       </c>
@@ -3876,10 +3876,10 @@
         <v>16</v>
       </c>
       <c r="I65" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>64</v>
       </c>
@@ -3896,10 +3896,10 @@
         <v>20</v>
       </c>
       <c r="I66" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>65</v>
       </c>
@@ -3919,7 +3919,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>66</v>
       </c>
@@ -3936,10 +3936,10 @@
         <v>75</v>
       </c>
       <c r="I68" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>67</v>
       </c>
@@ -3962,7 +3962,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>68</v>
       </c>
@@ -3985,12 +3985,12 @@
         <v>188</v>
       </c>
     </row>
-    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C71" t="s">
         <v>68</v>
@@ -4005,15 +4005,15 @@
         <v>75</v>
       </c>
       <c r="I71" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C72" t="s">
         <v>68</v>
@@ -4028,10 +4028,10 @@
         <v>75</v>
       </c>
       <c r="I72" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>71</v>
       </c>
@@ -4051,12 +4051,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C74" t="s">
         <v>68</v>
@@ -4065,13 +4065,13 @@
         <v>15</v>
       </c>
       <c r="F74" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I74" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>73</v>
       </c>
@@ -4091,7 +4091,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>74</v>
       </c>
@@ -4111,7 +4111,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>75</v>
       </c>
@@ -4131,7 +4131,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>76</v>
       </c>
@@ -4151,7 +4151,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>77</v>
       </c>
@@ -4174,7 +4174,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>78</v>
       </c>
@@ -4194,7 +4194,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="81" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>79</v>
       </c>
@@ -4214,7 +4214,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="82" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>80</v>
       </c>
@@ -4234,7 +4234,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>81</v>
       </c>
@@ -4254,10 +4254,10 @@
         <v>72</v>
       </c>
       <c r="I83" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>82</v>
       </c>
@@ -4277,7 +4277,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>83</v>
       </c>
@@ -4297,7 +4297,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="86" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>84</v>
       </c>
@@ -4314,15 +4314,15 @@
         <v>41</v>
       </c>
       <c r="I86" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C87" t="s">
         <v>68</v>
@@ -4334,13 +4334,13 @@
         <v>41</v>
       </c>
       <c r="F87" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I87" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>86</v>
       </c>
@@ -4360,10 +4360,10 @@
         <v>70</v>
       </c>
       <c r="I88" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>87</v>
       </c>
@@ -4380,13 +4380,13 @@
         <v>47</v>
       </c>
       <c r="F89" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="I89" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>88</v>
       </c>
@@ -4406,7 +4406,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>89</v>
       </c>
@@ -4426,7 +4426,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>90</v>
       </c>
@@ -4449,7 +4449,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>91</v>
       </c>
@@ -4469,7 +4469,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>92</v>
       </c>
@@ -4492,12 +4492,12 @@
         <v>142</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C95" t="s">
         <v>121</v>
@@ -4506,7 +4506,7 @@
         <v>11</v>
       </c>
       <c r="F95" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G95">
         <v>3</v>
@@ -4515,7 +4515,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>94</v>
       </c>
@@ -4529,7 +4529,7 @@
         <v>11</v>
       </c>
       <c r="F96" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G96">
         <v>3</v>
@@ -4541,12 +4541,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C97" t="s">
         <v>121</v>
@@ -4564,10 +4564,10 @@
         <v>3</v>
       </c>
       <c r="I97" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>96</v>
       </c>
@@ -4581,7 +4581,7 @@
         <v>11</v>
       </c>
       <c r="F98" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G98">
         <v>2</v>
@@ -4590,7 +4590,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>97</v>
       </c>
@@ -4604,7 +4604,7 @@
         <v>11</v>
       </c>
       <c r="F99" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="G99">
         <v>3</v>
@@ -4616,7 +4616,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>98</v>
       </c>
@@ -4642,7 +4642,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>99</v>
       </c>
@@ -4656,7 +4656,7 @@
         <v>11</v>
       </c>
       <c r="F101" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="G101">
         <v>3</v>
@@ -4668,7 +4668,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>100</v>
       </c>
@@ -4691,15 +4691,15 @@
         <v>4</v>
       </c>
       <c r="I102" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>101</v>
       </c>
       <c r="B103" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C103" t="s">
         <v>121</v>
@@ -4708,10 +4708,10 @@
         <v>15</v>
       </c>
       <c r="I103" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>102</v>
       </c>
@@ -4728,12 +4728,12 @@
         <v>204</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>103</v>
       </c>
       <c r="B105" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C105" t="s">
         <v>121</v>
@@ -4745,10 +4745,10 @@
         <v>16</v>
       </c>
       <c r="I105" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>104</v>
       </c>
@@ -4768,7 +4768,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>105</v>
       </c>
@@ -4788,7 +4788,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>106</v>
       </c>
@@ -4805,15 +4805,15 @@
         <v>20</v>
       </c>
       <c r="I108" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>107</v>
       </c>
       <c r="B109" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C109" t="s">
         <v>121</v>
@@ -4822,18 +4822,18 @@
         <v>15</v>
       </c>
       <c r="F109" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="I109" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>108</v>
       </c>
       <c r="B110" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C110" t="s">
         <v>121</v>
@@ -4845,18 +4845,18 @@
         <v>16</v>
       </c>
       <c r="F110" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="I110" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>109</v>
       </c>
       <c r="B111" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C111" t="s">
         <v>121</v>
@@ -4868,10 +4868,10 @@
         <v>137</v>
       </c>
       <c r="I111" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>110</v>
       </c>
@@ -4894,12 +4894,12 @@
         <v>156</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>111</v>
       </c>
       <c r="B113" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C113" t="s">
         <v>121</v>
@@ -4914,10 +4914,10 @@
         <v>137</v>
       </c>
       <c r="I113" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>112</v>
       </c>
@@ -4937,10 +4937,10 @@
         <v>137</v>
       </c>
       <c r="I114" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>113</v>
       </c>
@@ -4963,12 +4963,12 @@
         <v>140</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>114</v>
       </c>
       <c r="B116" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C116" t="s">
         <v>121</v>
@@ -4980,10 +4980,10 @@
         <v>31</v>
       </c>
       <c r="I116" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>115</v>
       </c>
@@ -5003,7 +5003,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>116</v>
       </c>
@@ -5023,7 +5023,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>117</v>
       </c>
@@ -5043,7 +5043,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>118</v>
       </c>
@@ -5063,12 +5063,12 @@
         <v>146</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>119</v>
       </c>
       <c r="B121" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C121" t="s">
         <v>121</v>
@@ -5080,15 +5080,15 @@
         <v>137</v>
       </c>
       <c r="I121" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>120</v>
       </c>
       <c r="B122" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C122" t="s">
         <v>121</v>
@@ -5100,15 +5100,15 @@
         <v>128</v>
       </c>
       <c r="I122" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>121</v>
       </c>
       <c r="B123" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C123" t="s">
         <v>121</v>
@@ -5123,15 +5123,15 @@
         <v>128</v>
       </c>
       <c r="I123" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>122</v>
       </c>
       <c r="B124" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C124" t="s">
         <v>121</v>
@@ -5149,7 +5149,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>123</v>
       </c>
@@ -5169,12 +5169,12 @@
         <v>148</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>124</v>
       </c>
       <c r="B126" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C126" t="s">
         <v>121</v>
@@ -5186,10 +5186,10 @@
         <v>130</v>
       </c>
       <c r="I126" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>125</v>
       </c>
@@ -5206,18 +5206,18 @@
         <v>20</v>
       </c>
       <c r="F127" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I127" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>126</v>
       </c>
       <c r="B128" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C128" t="s">
         <v>121</v>
@@ -5229,18 +5229,18 @@
         <v>20</v>
       </c>
       <c r="F128" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I128" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>127</v>
       </c>
       <c r="B129" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C129" t="s">
         <v>121</v>
@@ -5252,15 +5252,15 @@
         <v>137</v>
       </c>
       <c r="I129" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>128</v>
       </c>
       <c r="B130" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C130" t="s">
         <v>121</v>
@@ -5272,7 +5272,7 @@
         <v>128</v>
       </c>
       <c r="I130" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="131" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -5280,19 +5280,19 @@
         <v>129</v>
       </c>
       <c r="B131" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C131" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D131" t="s">
         <v>44</v>
       </c>
       <c r="F131" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I131" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="132" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -5300,19 +5300,19 @@
         <v>130</v>
       </c>
       <c r="B132" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C132" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D132" t="s">
         <v>44</v>
       </c>
       <c r="F132" t="s">
+        <v>241</v>
+      </c>
+      <c r="I132" t="s">
         <v>242</v>
-      </c>
-      <c r="I132" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="133" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -5320,10 +5320,10 @@
         <v>131</v>
       </c>
       <c r="B133" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C133" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D133" t="s">
         <v>11</v>
@@ -5340,10 +5340,10 @@
         <v>132</v>
       </c>
       <c r="B134" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C134" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D134" t="s">
         <v>11</v>
@@ -5355,7 +5355,7 @@
         <v>1</v>
       </c>
       <c r="I134" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="135" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -5363,10 +5363,10 @@
         <v>133</v>
       </c>
       <c r="B135" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C135" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D135" t="s">
         <v>11</v>
@@ -5378,7 +5378,7 @@
         <v>1</v>
       </c>
       <c r="I135" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="136" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -5386,16 +5386,16 @@
         <v>134</v>
       </c>
       <c r="B136" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C136" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D136" t="s">
         <v>11</v>
       </c>
       <c r="F136" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G136">
         <v>1</v>
@@ -5404,7 +5404,7 @@
         <v>2</v>
       </c>
       <c r="I136" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="137" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -5412,16 +5412,16 @@
         <v>135</v>
       </c>
       <c r="B137" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C137" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D137" t="s">
         <v>11</v>
       </c>
       <c r="F137" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G137">
         <v>1</v>
@@ -5430,7 +5430,7 @@
         <v>1</v>
       </c>
       <c r="I137" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="138" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -5438,16 +5438,16 @@
         <v>136</v>
       </c>
       <c r="B138" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C138" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D138" t="s">
         <v>11</v>
       </c>
       <c r="F138" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G138">
         <v>2</v>
@@ -5461,16 +5461,16 @@
         <v>137</v>
       </c>
       <c r="B139" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C139" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D139" t="s">
         <v>11</v>
       </c>
       <c r="F139" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G139">
         <v>3</v>
@@ -5479,7 +5479,7 @@
         <v>4</v>
       </c>
       <c r="I139" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="140" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -5487,16 +5487,16 @@
         <v>138</v>
       </c>
       <c r="B140" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C140" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D140" t="s">
         <v>11</v>
       </c>
       <c r="F140" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G140">
         <v>2</v>
@@ -5505,7 +5505,7 @@
         <v>3</v>
       </c>
       <c r="I140" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="141" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -5513,16 +5513,16 @@
         <v>139</v>
       </c>
       <c r="B141" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C141" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D141" t="s">
         <v>11</v>
       </c>
       <c r="F141" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G141">
         <v>2</v>
@@ -5531,7 +5531,7 @@
         <v>3</v>
       </c>
       <c r="I141" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="142" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -5539,16 +5539,16 @@
         <v>140</v>
       </c>
       <c r="B142" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C142" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D142" t="s">
         <v>11</v>
       </c>
       <c r="F142" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G142">
         <v>3</v>
@@ -5557,7 +5557,7 @@
         <v>3</v>
       </c>
       <c r="I142" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="143" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -5565,16 +5565,16 @@
         <v>141</v>
       </c>
       <c r="B143" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C143" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D143" t="s">
         <v>11</v>
       </c>
       <c r="F143" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G143">
         <v>3</v>
@@ -5583,7 +5583,7 @@
         <v>5</v>
       </c>
       <c r="I143" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="144" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -5591,16 +5591,16 @@
         <v>142</v>
       </c>
       <c r="B144" t="s">
+        <v>261</v>
+      </c>
+      <c r="C144" t="s">
+        <v>239</v>
+      </c>
+      <c r="D144" t="s">
+        <v>15</v>
+      </c>
+      <c r="I144" t="s">
         <v>262</v>
-      </c>
-      <c r="C144" t="s">
-        <v>240</v>
-      </c>
-      <c r="D144" t="s">
-        <v>15</v>
-      </c>
-      <c r="I144" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="145" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -5608,10 +5608,10 @@
         <v>143</v>
       </c>
       <c r="B145" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C145" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D145" t="s">
         <v>15</v>
@@ -5620,7 +5620,7 @@
         <v>16</v>
       </c>
       <c r="I145" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="146" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -5628,10 +5628,10 @@
         <v>144</v>
       </c>
       <c r="B146" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C146" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D146" t="s">
         <v>15</v>
@@ -5640,7 +5640,7 @@
         <v>16</v>
       </c>
       <c r="I146" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="147" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -5648,10 +5648,10 @@
         <v>145</v>
       </c>
       <c r="B147" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C147" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D147" t="s">
         <v>15</v>
@@ -5660,7 +5660,7 @@
         <v>16</v>
       </c>
       <c r="I147" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="148" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -5668,10 +5668,10 @@
         <v>146</v>
       </c>
       <c r="B148" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C148" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D148" t="s">
         <v>15</v>
@@ -5680,7 +5680,7 @@
         <v>47</v>
       </c>
       <c r="I148" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="149" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -5688,10 +5688,10 @@
         <v>147</v>
       </c>
       <c r="B149" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C149" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D149" t="s">
         <v>15</v>
@@ -5700,7 +5700,7 @@
         <v>31</v>
       </c>
       <c r="I149" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="150" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -5708,19 +5708,19 @@
         <v>148</v>
       </c>
       <c r="B150" t="s">
+        <v>266</v>
+      </c>
+      <c r="C150" t="s">
+        <v>239</v>
+      </c>
+      <c r="D150" t="s">
+        <v>15</v>
+      </c>
+      <c r="F150" t="s">
+        <v>249</v>
+      </c>
+      <c r="I150" t="s">
         <v>267</v>
-      </c>
-      <c r="C150" t="s">
-        <v>240</v>
-      </c>
-      <c r="D150" t="s">
-        <v>15</v>
-      </c>
-      <c r="F150" t="s">
-        <v>250</v>
-      </c>
-      <c r="I150" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="151" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -5728,16 +5728,16 @@
         <v>149</v>
       </c>
       <c r="B151" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C151" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D151" t="s">
         <v>15</v>
       </c>
       <c r="I151" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="152" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -5745,10 +5745,10 @@
         <v>150</v>
       </c>
       <c r="B152" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C152" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D152" t="s">
         <v>15</v>
@@ -5757,10 +5757,10 @@
         <v>20</v>
       </c>
       <c r="F152" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I152" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="153" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -5768,10 +5768,10 @@
         <v>151</v>
       </c>
       <c r="B153" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C153" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D153" t="s">
         <v>15</v>
@@ -5780,7 +5780,7 @@
         <v>20</v>
       </c>
       <c r="I153" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="154" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -5788,10 +5788,10 @@
         <v>152</v>
       </c>
       <c r="B154" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C154" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D154" t="s">
         <v>15</v>
@@ -5800,7 +5800,7 @@
         <v>47</v>
       </c>
       <c r="I154" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="155" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -5808,10 +5808,10 @@
         <v>153</v>
       </c>
       <c r="B155" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C155" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D155" t="s">
         <v>15</v>
@@ -5820,10 +5820,10 @@
         <v>31</v>
       </c>
       <c r="F155" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I155" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="156" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -5831,10 +5831,10 @@
         <v>154</v>
       </c>
       <c r="B156" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C156" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D156" t="s">
         <v>15</v>
@@ -5846,7 +5846,7 @@
         <v>17</v>
       </c>
       <c r="I156" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="157" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -5854,10 +5854,10 @@
         <v>155</v>
       </c>
       <c r="B157" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C157" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D157" t="s">
         <v>15</v>
@@ -5866,10 +5866,10 @@
         <v>16</v>
       </c>
       <c r="F157" t="s">
+        <v>360</v>
+      </c>
+      <c r="I157" t="s">
         <v>361</v>
-      </c>
-      <c r="I157" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="158" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -5877,19 +5877,19 @@
         <v>156</v>
       </c>
       <c r="B158" t="s">
+        <v>263</v>
+      </c>
+      <c r="C158" t="s">
+        <v>239</v>
+      </c>
+      <c r="D158" t="s">
+        <v>15</v>
+      </c>
+      <c r="F158" t="s">
+        <v>255</v>
+      </c>
+      <c r="I158" t="s">
         <v>264</v>
-      </c>
-      <c r="C158" t="s">
-        <v>240</v>
-      </c>
-      <c r="D158" t="s">
-        <v>15</v>
-      </c>
-      <c r="F158" t="s">
-        <v>256</v>
-      </c>
-      <c r="I158" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="159" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -5897,19 +5897,19 @@
         <v>157</v>
       </c>
       <c r="B159" t="s">
+        <v>268</v>
+      </c>
+      <c r="C159" t="s">
+        <v>239</v>
+      </c>
+      <c r="D159" t="s">
+        <v>15</v>
+      </c>
+      <c r="F159" t="s">
+        <v>255</v>
+      </c>
+      <c r="I159" t="s">
         <v>269</v>
-      </c>
-      <c r="C159" t="s">
-        <v>240</v>
-      </c>
-      <c r="D159" t="s">
-        <v>15</v>
-      </c>
-      <c r="F159" t="s">
-        <v>256</v>
-      </c>
-      <c r="I159" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="160" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -5917,10 +5917,10 @@
         <v>158</v>
       </c>
       <c r="B160" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C160" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D160" t="s">
         <v>15</v>
@@ -5929,10 +5929,10 @@
         <v>47</v>
       </c>
       <c r="F160" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I160" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="161" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -5940,10 +5940,10 @@
         <v>159</v>
       </c>
       <c r="B161" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C161" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D161" t="s">
         <v>15</v>
@@ -5952,10 +5952,10 @@
         <v>47</v>
       </c>
       <c r="F161" t="s">
+        <v>364</v>
+      </c>
+      <c r="I161" t="s">
         <v>365</v>
-      </c>
-      <c r="I161" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="162" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -5963,10 +5963,10 @@
         <v>160</v>
       </c>
       <c r="B162" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C162" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D162" t="s">
         <v>15</v>
@@ -5975,10 +5975,10 @@
         <v>31</v>
       </c>
       <c r="F162" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I162" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="163" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -5986,16 +5986,16 @@
         <v>161</v>
       </c>
       <c r="B163" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C163" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D163" t="s">
         <v>27</v>
       </c>
       <c r="I163" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="164" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -6003,16 +6003,16 @@
         <v>162</v>
       </c>
       <c r="B164" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C164" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D164" t="s">
         <v>27</v>
       </c>
       <c r="I164" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="165" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -6020,16 +6020,16 @@
         <v>163</v>
       </c>
       <c r="B165" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C165" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D165" t="s">
         <v>27</v>
       </c>
       <c r="I165" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="166" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -6037,10 +6037,10 @@
         <v>164</v>
       </c>
       <c r="B166" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C166" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D166" t="s">
         <v>27</v>
@@ -6054,19 +6054,19 @@
         <v>165</v>
       </c>
       <c r="B167" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C167" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D167" t="s">
         <v>44</v>
       </c>
       <c r="F167" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I167" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="168" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -6074,10 +6074,10 @@
         <v>166</v>
       </c>
       <c r="B168" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C168" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D168" t="s">
         <v>11</v>
@@ -6094,14 +6094,17 @@
         <v>167</v>
       </c>
       <c r="B169" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C169" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D169" t="s">
         <v>11</v>
       </c>
+      <c r="F169" t="s">
+        <v>393</v>
+      </c>
       <c r="G169">
         <v>1</v>
       </c>
@@ -6109,7 +6112,7 @@
         <v>1</v>
       </c>
       <c r="I169" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="170" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -6117,10 +6120,10 @@
         <v>168</v>
       </c>
       <c r="B170" t="s">
+        <v>295</v>
+      </c>
+      <c r="C170" t="s">
         <v>296</v>
-      </c>
-      <c r="C170" t="s">
-        <v>297</v>
       </c>
       <c r="D170" t="s">
         <v>11</v>
@@ -6132,7 +6135,7 @@
         <v>1</v>
       </c>
       <c r="I170" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="171" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -6140,16 +6143,16 @@
         <v>169</v>
       </c>
       <c r="B171" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C171" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D171" t="s">
         <v>11</v>
       </c>
       <c r="F171" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G171">
         <v>2</v>
@@ -6158,7 +6161,7 @@
         <v>2</v>
       </c>
       <c r="I171" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="172" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -6166,10 +6169,10 @@
         <v>170</v>
       </c>
       <c r="B172" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C172" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D172" t="s">
         <v>11</v>
@@ -6181,7 +6184,7 @@
         <v>2</v>
       </c>
       <c r="I172" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="173" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -6189,16 +6192,16 @@
         <v>171</v>
       </c>
       <c r="B173" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C173" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D173" t="s">
         <v>11</v>
       </c>
       <c r="F173" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G173">
         <v>2</v>
@@ -6207,7 +6210,7 @@
         <v>3</v>
       </c>
       <c r="I173" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="174" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -6215,16 +6218,16 @@
         <v>172</v>
       </c>
       <c r="B174" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C174" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D174" t="s">
         <v>11</v>
       </c>
       <c r="F174" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G174">
         <v>3</v>
@@ -6233,7 +6236,7 @@
         <v>3</v>
       </c>
       <c r="I174" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="175" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -6241,16 +6244,16 @@
         <v>173</v>
       </c>
       <c r="B175" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C175" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D175" t="s">
         <v>11</v>
       </c>
       <c r="F175" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G175">
         <v>4</v>
@@ -6259,7 +6262,7 @@
         <v>4</v>
       </c>
       <c r="I175" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="176" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -6267,16 +6270,16 @@
         <v>174</v>
       </c>
       <c r="B176" t="s">
+        <v>325</v>
+      </c>
+      <c r="C176" t="s">
+        <v>296</v>
+      </c>
+      <c r="D176" t="s">
+        <v>15</v>
+      </c>
+      <c r="I176" t="s">
         <v>326</v>
-      </c>
-      <c r="C176" t="s">
-        <v>297</v>
-      </c>
-      <c r="D176" t="s">
-        <v>15</v>
-      </c>
-      <c r="I176" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="177" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -6284,16 +6287,16 @@
         <v>175</v>
       </c>
       <c r="B177" t="s">
+        <v>310</v>
+      </c>
+      <c r="C177" t="s">
+        <v>296</v>
+      </c>
+      <c r="D177" t="s">
+        <v>15</v>
+      </c>
+      <c r="I177" t="s">
         <v>311</v>
-      </c>
-      <c r="C177" t="s">
-        <v>297</v>
-      </c>
-      <c r="D177" t="s">
-        <v>15</v>
-      </c>
-      <c r="I177" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="178" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -6301,16 +6304,16 @@
         <v>176</v>
       </c>
       <c r="B178" t="s">
+        <v>313</v>
+      </c>
+      <c r="C178" t="s">
+        <v>296</v>
+      </c>
+      <c r="D178" t="s">
+        <v>15</v>
+      </c>
+      <c r="I178" t="s">
         <v>314</v>
-      </c>
-      <c r="C178" t="s">
-        <v>297</v>
-      </c>
-      <c r="D178" t="s">
-        <v>15</v>
-      </c>
-      <c r="I178" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="179" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -6318,16 +6321,16 @@
         <v>177</v>
       </c>
       <c r="B179" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C179" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D179" t="s">
         <v>15</v>
       </c>
       <c r="I179" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="180" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -6335,10 +6338,10 @@
         <v>178</v>
       </c>
       <c r="B180" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C180" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D180" t="s">
         <v>15</v>
@@ -6347,10 +6350,10 @@
         <v>47</v>
       </c>
       <c r="F180" t="s">
+        <v>390</v>
+      </c>
+      <c r="I180" t="s">
         <v>391</v>
-      </c>
-      <c r="I180" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="181" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -6358,19 +6361,19 @@
         <v>179</v>
       </c>
       <c r="B181" t="s">
+        <v>319</v>
+      </c>
+      <c r="C181" t="s">
+        <v>296</v>
+      </c>
+      <c r="D181" t="s">
+        <v>15</v>
+      </c>
+      <c r="F181" t="s">
+        <v>298</v>
+      </c>
+      <c r="I181" t="s">
         <v>320</v>
-      </c>
-      <c r="C181" t="s">
-        <v>297</v>
-      </c>
-      <c r="D181" t="s">
-        <v>15</v>
-      </c>
-      <c r="F181" t="s">
-        <v>299</v>
-      </c>
-      <c r="I181" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="182" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -6378,19 +6381,19 @@
         <v>180</v>
       </c>
       <c r="B182" t="s">
+        <v>331</v>
+      </c>
+      <c r="C182" t="s">
+        <v>296</v>
+      </c>
+      <c r="D182" t="s">
+        <v>15</v>
+      </c>
+      <c r="F182" t="s">
+        <v>393</v>
+      </c>
+      <c r="I182" t="s">
         <v>332</v>
-      </c>
-      <c r="C182" t="s">
-        <v>297</v>
-      </c>
-      <c r="D182" t="s">
-        <v>15</v>
-      </c>
-      <c r="F182" t="s">
-        <v>394</v>
-      </c>
-      <c r="I182" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="183" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -6398,19 +6401,19 @@
         <v>181</v>
       </c>
       <c r="B183" t="s">
+        <v>315</v>
+      </c>
+      <c r="C183" t="s">
+        <v>296</v>
+      </c>
+      <c r="D183" t="s">
+        <v>15</v>
+      </c>
+      <c r="F183" t="s">
+        <v>298</v>
+      </c>
+      <c r="I183" t="s">
         <v>316</v>
-      </c>
-      <c r="C183" t="s">
-        <v>297</v>
-      </c>
-      <c r="D183" t="s">
-        <v>15</v>
-      </c>
-      <c r="F183" t="s">
-        <v>299</v>
-      </c>
-      <c r="I183" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="184" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -6418,10 +6421,10 @@
         <v>182</v>
       </c>
       <c r="B184" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C184" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D184" t="s">
         <v>15</v>
@@ -6430,10 +6433,10 @@
         <v>16</v>
       </c>
       <c r="F184" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I184" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="185" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -6441,10 +6444,10 @@
         <v>183</v>
       </c>
       <c r="B185" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C185" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D185" t="s">
         <v>15</v>
@@ -6453,10 +6456,10 @@
         <v>20</v>
       </c>
       <c r="F185" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I185" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="186" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -6464,10 +6467,10 @@
         <v>184</v>
       </c>
       <c r="B186" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C186" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D186" t="s">
         <v>15</v>
@@ -6476,7 +6479,7 @@
         <v>47</v>
       </c>
       <c r="I186" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="187" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -6484,10 +6487,10 @@
         <v>185</v>
       </c>
       <c r="B187" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C187" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D187" t="s">
         <v>15</v>
@@ -6496,10 +6499,10 @@
         <v>16</v>
       </c>
       <c r="F187" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I187" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="188" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -6507,10 +6510,10 @@
         <v>186</v>
       </c>
       <c r="B188" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C188" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D188" t="s">
         <v>15</v>
@@ -6519,10 +6522,10 @@
         <v>47</v>
       </c>
       <c r="F188" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I188" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="189" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -6530,10 +6533,10 @@
         <v>187</v>
       </c>
       <c r="B189" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C189" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D189" t="s">
         <v>15</v>
@@ -6542,10 +6545,10 @@
         <v>20</v>
       </c>
       <c r="F189" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I189" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="190" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -6553,19 +6556,19 @@
         <v>188</v>
       </c>
       <c r="B190" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C190" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D190" t="s">
         <v>15</v>
       </c>
       <c r="F190" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="I190" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="191" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -6573,19 +6576,19 @@
         <v>189</v>
       </c>
       <c r="B191" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C191" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D191" t="s">
         <v>15</v>
       </c>
       <c r="F191" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I191" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="192" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -6593,10 +6596,10 @@
         <v>190</v>
       </c>
       <c r="B192" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C192" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D192" t="s">
         <v>27</v>
@@ -6605,12 +6608,12 @@
         <v>41</v>
       </c>
       <c r="I192" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:F1048576">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>$J$1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Colour images and add images up to 249
</commit_message>
<xml_diff>
--- a/design/cards.xlsx
+++ b/design/cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zoey\git\hexal-ccg\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8CB0D2E6-5396-4D61-9457-43D6608EF0FE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0CBB20A-860F-41D2-8CD3-574303CF6D8A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="228" yWindow="468" windowWidth="30588" windowHeight="19836" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12" yWindow="0" windowWidth="23016" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cards" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1242" uniqueCount="528">
   <si>
     <t>ID</t>
   </si>
@@ -1357,9 +1357,6 @@
     <t>When this is attacked and destroyed by an enemy creature, destroy that creature.</t>
   </si>
   <si>
-    <t>Poisonous Frog</t>
-  </si>
-  <si>
     <t>Gifted Wanderer</t>
   </si>
   <si>
@@ -1525,9 +1522,6 @@
     <t>Spirit Militia</t>
   </si>
   <si>
-    <t>Guardian Stones</t>
-  </si>
-  <si>
     <t>Manifest Dreams</t>
   </si>
   <si>
@@ -1589,6 +1583,42 @@
   </si>
   <si>
     <t>Seal World Line</t>
+  </si>
+  <si>
+    <t>Poisonous Bee</t>
+  </si>
+  <si>
+    <t>Haunted Wine Glass</t>
+  </si>
+  <si>
+    <t>At the start of your turn you may destroy this to summon a [Spirit] creature with cost 0 from your hand. Give it &lt;ready&gt;.</t>
+  </si>
+  <si>
+    <t>Guardian Stone</t>
+  </si>
+  <si>
+    <t>Reveal the top card of your opponent's deck. If it's a spell, draw a card.</t>
+  </si>
+  <si>
+    <t>Spell Scroll</t>
+  </si>
+  <si>
+    <t>&lt;Search&gt; for a spell. Replace it with this card.</t>
+  </si>
+  <si>
+    <t>Peek</t>
+  </si>
+  <si>
+    <t>Smudge Stick</t>
+  </si>
+  <si>
+    <t>Destroy all tokens.</t>
+  </si>
+  <si>
+    <t>Equip to a friendly creature. It gains +1 / +0 and "can attack creatures with &lt;ethereal&gt;".</t>
+  </si>
+  <si>
+    <t>Ethereal Dagger</t>
   </si>
 </sst>
 </file>
@@ -2647,8 +2677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I251"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A221" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E251" sqref="E251"/>
+    <sheetView tabSelected="1" topLeftCell="A243" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B252" sqref="B252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4159,7 +4189,7 @@
         <v>16</v>
       </c>
       <c r="I65" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
@@ -6088,7 +6118,7 @@
         <v>206</v>
       </c>
       <c r="I152" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.3">
@@ -6607,7 +6637,7 @@
         <v>15</v>
       </c>
       <c r="I176" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.3">
@@ -6807,7 +6837,7 @@
         <v>45</v>
       </c>
       <c r="I186" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.3">
@@ -6830,7 +6860,7 @@
         <v>248</v>
       </c>
       <c r="I187" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.3">
@@ -6939,7 +6969,7 @@
         <v>246</v>
       </c>
       <c r="I192" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.3">
@@ -7263,7 +7293,7 @@
         <v>205</v>
       </c>
       <c r="B207" t="s">
-        <v>440</v>
+        <v>516</v>
       </c>
       <c r="C207" t="s">
         <v>106</v>
@@ -7289,7 +7319,7 @@
         <v>206</v>
       </c>
       <c r="B208" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C208" t="s">
         <v>106</v>
@@ -7312,7 +7342,7 @@
         <v>207</v>
       </c>
       <c r="B209" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C209" t="s">
         <v>106</v>
@@ -7338,7 +7368,7 @@
         <v>208</v>
       </c>
       <c r="B210" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C210" t="s">
         <v>106</v>
@@ -7361,7 +7391,7 @@
         <v>209</v>
       </c>
       <c r="B211" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C211" t="s">
         <v>106</v>
@@ -7373,7 +7403,7 @@
         <v>16</v>
       </c>
       <c r="I211" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.3">
@@ -7381,7 +7411,7 @@
         <v>210</v>
       </c>
       <c r="B212" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C212" t="s">
         <v>106</v>
@@ -7396,7 +7426,7 @@
         <v>119</v>
       </c>
       <c r="I212" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.3">
@@ -7404,7 +7434,7 @@
         <v>211</v>
       </c>
       <c r="B213" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C213" t="s">
         <v>106</v>
@@ -7416,7 +7446,7 @@
         <v>40</v>
       </c>
       <c r="I213" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.3">
@@ -7424,7 +7454,7 @@
         <v>212</v>
       </c>
       <c r="B214" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C214" t="s">
         <v>106</v>
@@ -7433,7 +7463,7 @@
         <v>26</v>
       </c>
       <c r="I214" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.3">
@@ -7441,7 +7471,7 @@
         <v>213</v>
       </c>
       <c r="B215" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C215" t="s">
         <v>106</v>
@@ -7456,7 +7486,7 @@
         <v>111</v>
       </c>
       <c r="I215" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.3">
@@ -7464,7 +7494,7 @@
         <v>214</v>
       </c>
       <c r="B216" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C216" t="s">
         <v>196</v>
@@ -7479,7 +7509,7 @@
         <v>1</v>
       </c>
       <c r="I216" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.3">
@@ -7487,7 +7517,7 @@
         <v>215</v>
       </c>
       <c r="B217" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C217" t="s">
         <v>196</v>
@@ -7505,7 +7535,7 @@
         <v>2</v>
       </c>
       <c r="I217" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.3">
@@ -7513,7 +7543,7 @@
         <v>216</v>
       </c>
       <c r="B218" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C218" t="s">
         <v>196</v>
@@ -7528,7 +7558,7 @@
         <v>2</v>
       </c>
       <c r="I218" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="219" spans="1:9" x14ac:dyDescent="0.3">
@@ -7536,7 +7566,7 @@
         <v>217</v>
       </c>
       <c r="B219" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C219" t="s">
         <v>196</v>
@@ -7562,7 +7592,7 @@
         <v>218</v>
       </c>
       <c r="B220" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C220" t="s">
         <v>196</v>
@@ -7574,7 +7604,7 @@
         <v>206</v>
       </c>
       <c r="I220" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="221" spans="1:9" x14ac:dyDescent="0.3">
@@ -7582,7 +7612,7 @@
         <v>219</v>
       </c>
       <c r="B221" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C221" t="s">
         <v>196</v>
@@ -7597,7 +7627,7 @@
         <v>206</v>
       </c>
       <c r="I221" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.3">
@@ -7605,7 +7635,7 @@
         <v>220</v>
       </c>
       <c r="B222" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C222" t="s">
         <v>196</v>
@@ -7625,7 +7655,7 @@
         <v>221</v>
       </c>
       <c r="B223" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C223" t="s">
         <v>196</v>
@@ -7640,7 +7670,7 @@
         <v>206</v>
       </c>
       <c r="I223" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.3">
@@ -7648,7 +7678,7 @@
         <v>222</v>
       </c>
       <c r="B224" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C224" t="s">
         <v>196</v>
@@ -7663,7 +7693,7 @@
         <v>346</v>
       </c>
       <c r="I224" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="225" spans="1:9" x14ac:dyDescent="0.3">
@@ -7671,7 +7701,7 @@
         <v>223</v>
       </c>
       <c r="B225" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C225" t="s">
         <v>196</v>
@@ -7683,7 +7713,7 @@
         <v>40</v>
       </c>
       <c r="I225" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="226" spans="1:9" x14ac:dyDescent="0.3">
@@ -7691,7 +7721,7 @@
         <v>224</v>
       </c>
       <c r="B226" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C226" t="s">
         <v>196</v>
@@ -7703,7 +7733,7 @@
         <v>206</v>
       </c>
       <c r="I226" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="227" spans="1:9" x14ac:dyDescent="0.3">
@@ -7711,7 +7741,7 @@
         <v>225</v>
       </c>
       <c r="B227" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C227" t="s">
         <v>196</v>
@@ -7723,7 +7753,7 @@
         <v>206</v>
       </c>
       <c r="I227" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.3">
@@ -7731,7 +7761,7 @@
         <v>226</v>
       </c>
       <c r="B228" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C228" t="s">
         <v>244</v>
@@ -7743,7 +7773,7 @@
         <v>280</v>
       </c>
       <c r="I228" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.3">
@@ -7751,7 +7781,7 @@
         <v>227</v>
       </c>
       <c r="B229" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C229" t="s">
         <v>244</v>
@@ -7766,7 +7796,7 @@
         <v>328</v>
       </c>
       <c r="I229" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="230" spans="1:9" x14ac:dyDescent="0.3">
@@ -7774,7 +7804,7 @@
         <v>228</v>
       </c>
       <c r="B230" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C230" t="s">
         <v>244</v>
@@ -7786,7 +7816,7 @@
         <v>40</v>
       </c>
       <c r="I230" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="231" spans="1:9" x14ac:dyDescent="0.3">
@@ -7794,7 +7824,7 @@
         <v>229</v>
       </c>
       <c r="B231" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C231" t="s">
         <v>244</v>
@@ -7809,7 +7839,7 @@
         <v>1</v>
       </c>
       <c r="I231" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="232" spans="1:9" x14ac:dyDescent="0.3">
@@ -7817,7 +7847,7 @@
         <v>230</v>
       </c>
       <c r="B232" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C232" t="s">
         <v>244</v>
@@ -7832,7 +7862,7 @@
         <v>2</v>
       </c>
       <c r="I232" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.3">
@@ -7840,7 +7870,7 @@
         <v>231</v>
       </c>
       <c r="B233" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C233" t="s">
         <v>244</v>
@@ -7855,7 +7885,7 @@
         <v>2</v>
       </c>
       <c r="I233" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="234" spans="1:9" x14ac:dyDescent="0.3">
@@ -7863,7 +7893,7 @@
         <v>232</v>
       </c>
       <c r="B234" t="s">
-        <v>496</v>
+        <v>519</v>
       </c>
       <c r="C234" t="s">
         <v>244</v>
@@ -7886,7 +7916,7 @@
         <v>233</v>
       </c>
       <c r="B235" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C235" t="s">
         <v>244</v>
@@ -7904,7 +7934,7 @@
         <v>1</v>
       </c>
       <c r="I235" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="236" spans="1:9" x14ac:dyDescent="0.3">
@@ -7912,7 +7942,7 @@
         <v>234</v>
       </c>
       <c r="B236" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C236" t="s">
         <v>244</v>
@@ -7930,7 +7960,7 @@
         <v>2</v>
       </c>
       <c r="I236" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="237" spans="1:9" x14ac:dyDescent="0.3">
@@ -7938,7 +7968,7 @@
         <v>235</v>
       </c>
       <c r="B237" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C237" t="s">
         <v>244</v>
@@ -7961,7 +7991,7 @@
         <v>236</v>
       </c>
       <c r="B238" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C238" t="s">
         <v>244</v>
@@ -7973,7 +8003,7 @@
         <v>324</v>
       </c>
       <c r="I238" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="239" spans="1:9" x14ac:dyDescent="0.3">
@@ -7981,7 +8011,7 @@
         <v>237</v>
       </c>
       <c r="B239" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C239" t="s">
         <v>244</v>
@@ -7993,7 +8023,7 @@
         <v>328</v>
       </c>
       <c r="I239" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="240" spans="1:9" x14ac:dyDescent="0.3">
@@ -8001,7 +8031,7 @@
         <v>238</v>
       </c>
       <c r="B240" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C240" t="s">
         <v>244</v>
@@ -8010,7 +8040,7 @@
         <v>15</v>
       </c>
       <c r="I240" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="241" spans="1:9" x14ac:dyDescent="0.3">
@@ -8018,7 +8048,7 @@
         <v>239</v>
       </c>
       <c r="B241" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C241" t="s">
         <v>244</v>
@@ -8027,7 +8057,7 @@
         <v>15</v>
       </c>
       <c r="I241" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="242" spans="1:9" x14ac:dyDescent="0.3">
@@ -8035,7 +8065,7 @@
         <v>240</v>
       </c>
       <c r="B242" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="C242" t="s">
         <v>244</v>
@@ -8047,7 +8077,7 @@
         <v>371</v>
       </c>
       <c r="I242" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="243" spans="1:9" x14ac:dyDescent="0.3">
@@ -8055,7 +8085,7 @@
         <v>241</v>
       </c>
       <c r="B243" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C243" t="s">
         <v>244</v>
@@ -8070,7 +8100,7 @@
         <v>328</v>
       </c>
       <c r="I243" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="244" spans="1:9" x14ac:dyDescent="0.3">
@@ -8078,7 +8108,7 @@
         <v>242</v>
       </c>
       <c r="B244" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="C244" t="s">
         <v>244</v>
@@ -8093,7 +8123,7 @@
         <v>248</v>
       </c>
       <c r="I244" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="245" spans="1:9" x14ac:dyDescent="0.3">
@@ -8101,7 +8131,7 @@
         <v>243</v>
       </c>
       <c r="B245" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="C245" t="s">
         <v>244</v>
@@ -8113,62 +8143,101 @@
         <v>45</v>
       </c>
       <c r="I245" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="246" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>244</v>
       </c>
+      <c r="B246" t="s">
+        <v>515</v>
+      </c>
       <c r="C246" t="s">
         <v>244</v>
       </c>
       <c r="D246" t="s">
-        <v>26</v>
+        <v>15</v>
+      </c>
+      <c r="E246" t="s">
+        <v>45</v>
+      </c>
+      <c r="I246" t="s">
+        <v>514</v>
       </c>
     </row>
     <row r="247" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>245</v>
       </c>
+      <c r="B247" t="s">
+        <v>517</v>
+      </c>
       <c r="C247" t="s">
         <v>244</v>
       </c>
       <c r="D247" t="s">
         <v>26</v>
+      </c>
+      <c r="E247" t="s">
+        <v>45</v>
+      </c>
+      <c r="I247" t="s">
+        <v>518</v>
       </c>
     </row>
     <row r="248" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>246</v>
       </c>
+      <c r="B248" t="s">
+        <v>523</v>
+      </c>
       <c r="C248" t="s">
         <v>244</v>
       </c>
       <c r="D248" t="s">
         <v>26</v>
+      </c>
+      <c r="I248" t="s">
+        <v>520</v>
       </c>
     </row>
     <row r="249" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>247</v>
       </c>
+      <c r="B249" t="s">
+        <v>521</v>
+      </c>
       <c r="C249" t="s">
         <v>244</v>
       </c>
       <c r="D249" t="s">
         <v>26</v>
+      </c>
+      <c r="I249" t="s">
+        <v>522</v>
       </c>
     </row>
     <row r="250" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>248</v>
       </c>
+      <c r="B250" t="s">
+        <v>524</v>
+      </c>
       <c r="C250" t="s">
         <v>244</v>
       </c>
       <c r="D250" t="s">
         <v>26</v>
+      </c>
+      <c r="F250" t="s">
+        <v>335</v>
+      </c>
+      <c r="I250" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="251" spans="1:9" x14ac:dyDescent="0.3">
@@ -8176,19 +8245,25 @@
         <v>249</v>
       </c>
       <c r="B251" t="s">
-        <v>517</v>
+        <v>527</v>
       </c>
       <c r="C251" t="s">
         <v>244</v>
       </c>
       <c r="D251" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="E251" t="s">
-        <v>45</v>
+        <v>40</v>
+      </c>
+      <c r="G251">
+        <v>1</v>
+      </c>
+      <c r="H251">
+        <v>0</v>
       </c>
       <c r="I251" t="s">
-        <v>516</v>
+        <v>526</v>
       </c>
     </row>
   </sheetData>

</xml_diff>